<commit_message>
Added inspection over the required files
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1. Repositories\VVSS_Tasks\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D42F2A60-65E4-45A9-8979-25B06295C9EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64078D71-09FB-4166-A047-AA0DD41D527E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="85">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -132,13 +132,173 @@
     <t>Tool-based Code Analysis</t>
   </si>
   <si>
-    <t>Effort to perform tool-based code analysis (hours):</t>
-  </si>
-  <si>
     <t>Mogage Nicolae</t>
   </si>
   <si>
     <t>Moldovan Denis-Angel</t>
+  </si>
+  <si>
+    <t>R01</t>
+  </si>
+  <si>
+    <t>R02</t>
+  </si>
+  <si>
+    <t>R05</t>
+  </si>
+  <si>
+    <t>F03</t>
+  </si>
+  <si>
+    <t>Nu este precizat ce informații ale unui anumit task să fie afișate</t>
+  </si>
+  <si>
+    <t>F04</t>
+  </si>
+  <si>
+    <t>F02</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Nu se specifică tipul de aplicație care va fi dezvoltată.</t>
+  </si>
+  <si>
+    <t>Trebuie precizat ce detalii de doresc modificate in aceasta functie. Nu se specifică cum se face interacțiunea cu interfața.</t>
+  </si>
+  <si>
+    <t>A01</t>
+  </si>
+  <si>
+    <t>A02</t>
+  </si>
+  <si>
+    <t>A03</t>
+  </si>
+  <si>
+    <t>A05</t>
+  </si>
+  <si>
+    <t>A06</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>yes, e arhitectura mvc</t>
+  </si>
+  <si>
+    <t>se folosește logger pentru afisarea erorilor, dar nu există niciun mecanism în cazul în care o funcție dă eroare</t>
+  </si>
+  <si>
+    <t>se folosește mvc si observer</t>
+  </si>
+  <si>
+    <t>Clasa Task</t>
+  </si>
+  <si>
+    <t>In cerințe de precizează să fie descrierea, data și ora de început, data și ora de final, iar daca task-ul este repetitiv, și numărul de ore și minute la care se repetă, însă Task are doar doi contructori care, unul accepta doar o descriere și o dată, celalalt acceptând o descriere 2 date și un număr întreg, nefiind respectate cerințele</t>
+  </si>
+  <si>
+    <t>C06</t>
+  </si>
+  <si>
+    <t>DateService -&gt; linia 31</t>
+  </si>
+  <si>
+    <t>Pentru cazul în care nu se specifică timpul în aplicație la filtrare, va determina o eroare de tip NumberFormatException, neputând parsa un string gol</t>
+  </si>
+  <si>
+    <t>C08</t>
+  </si>
+  <si>
+    <t>Nu exista bro</t>
+  </si>
+  <si>
+    <t>C07</t>
+  </si>
+  <si>
+    <t>Există log-uri în cazurile de eroare</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>C01</t>
+  </si>
+  <si>
+    <t>Nu se fac actualizările și în service pentru delete</t>
+  </si>
+  <si>
+    <t>Controller -&gt; linia 108</t>
+  </si>
+  <si>
+    <t>DateService.java, linia 34</t>
+  </si>
+  <si>
+    <t>DateService.java, linia 41</t>
+  </si>
+  <si>
+    <t>Use static access with "java.util.Calendar" for "getInstance"</t>
+  </si>
+  <si>
+    <t>Calendar calendar = GregorianCalendar.getInstance();</t>
+  </si>
+  <si>
+    <t>Calendar calendar = Calendar.getInstance();</t>
+  </si>
+  <si>
+    <t>NewEditController, linia 79</t>
+  </si>
+  <si>
+    <t>Add a default case to this switch</t>
+  </si>
+  <si>
+    <t>switch (clickedButton.getId()){
+case "btnNew" : initNewWindow("New Task");
+break;
+case "btnEdit" : initEditWindow("Edit Task");
+break;}</t>
+  </si>
+  <si>
+    <t>switch (clickedButton.getId()){
+case "btnNew" : initNewWindow("New Task");
+break;
+case "btnEdit" : initEditWindow("Edit Task");
+break;
+default: log.error("no button was clicked");}</t>
+  </si>
+  <si>
+    <t>TasksService, linia 51</t>
+  </si>
+  <si>
+    <t>This block of commented-out lines of code should be removed</t>
+  </si>
+  <si>
+    <t>//Iterable&lt;Task&gt; filtered = tasks.incoming(start, end);</t>
+  </si>
+  <si>
+    <t>TasksService, linia 44</t>
+  </si>
+  <si>
+    <t>int result = (hours * DateService.MINUTES_IN_HOUR + minutes) * DateService.SECONDS_IN_MINUTE;
+return result;</t>
+  </si>
+  <si>
+    <t>return (hours * DateService.MINUTES_IN_HOUR + minutes) * DateService.SECONDS_IN_MINUTE;</t>
+  </si>
+  <si>
+    <t>SonarLint</t>
+  </si>
+  <si>
+    <t>19.03.2024</t>
+  </si>
+  <si>
+    <t>Immediately return this expression instead of assigning it to the temporary variable "result"</t>
+  </si>
+  <si>
+    <t>Nicolae Mogage</t>
   </si>
 </sst>
 </file>
@@ -257,7 +417,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -321,16 +481,33 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -352,14 +529,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -396,13 +571,42 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -710,10 +914,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:J4"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,21 +951,21 @@
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="16" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="17">
+      <c r="I3" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="16">
         <v>234</v>
       </c>
     </row>
@@ -773,11 +977,11 @@
         <v>14</v>
       </c>
       <c r="E4" s="24"/>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="35" t="s">
-        <v>34</v>
+      <c r="I4" s="20" t="s">
+        <v>33</v>
       </c>
       <c r="J4" s="3">
         <v>234</v>
@@ -791,7 +995,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="26"/>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
@@ -802,14 +1006,18 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
+      <c r="D6" s="21" t="s">
+        <v>84</v>
+      </c>
       <c r="E6" s="21"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
+      <c r="D7" s="21" t="s">
+        <v>82</v>
+      </c>
       <c r="E7" s="21"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -826,158 +1034,193 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="2"/>
+      <c r="C10" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="38"/>
+      <c r="D11" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="40"/>
+    </row>
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
-        <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
-        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
+      <c r="C13" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="39" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B14:B26" si="0">B13+1</f>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="2"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="40"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="2"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="34"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="2"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="34"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="2"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="34"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="15"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="34"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="15"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="36"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="15"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="36"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="15"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="36"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="15"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="36"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="15"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="36"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="15"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="36"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="15"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C27" s="11" t="s">
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="36"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="3">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="36"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C28" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="12"/>
-      <c r="E27" s="1"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="1">
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="10">
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C13:C14"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="B2:E2"/>
@@ -995,10 +1238,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,21 +1274,21 @@
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="16" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="17">
+      <c r="I3" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="16">
         <v>234</v>
       </c>
     </row>
@@ -1057,11 +1300,11 @@
         <v>15</v>
       </c>
       <c r="E4" s="27"/>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="35" t="s">
-        <v>34</v>
+      <c r="I4" s="20" t="s">
+        <v>33</v>
       </c>
       <c r="J4" s="3">
         <v>234</v>
@@ -1075,7 +1318,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="29"/>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
@@ -1093,7 +1336,9 @@
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
+      <c r="D7" s="21" t="s">
+        <v>82</v>
+      </c>
       <c r="E7" s="21"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1114,160 +1359,199 @@
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="C10" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
-        <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
-        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
+      <c r="C13" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B14:B27" si="0">B13+1</f>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="C14" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="34" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="2"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="34"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="2"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="44"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="2"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="2"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="44"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="2"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="44"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="2"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="44"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="2"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="44"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="2"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="44"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="2"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C28" s="11" t="s">
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="44"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="3">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C29" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="12"/>
-      <c r="E28" s="1"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="1">
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1291,7 +1575,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:J4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1299,7 +1583,7 @@
     <col min="1" max="1" width="8.85546875" style="6"/>
     <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="18" style="6" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" style="6" customWidth="1"/>
     <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
     <col min="6" max="8" width="8.85546875" style="6"/>
     <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
@@ -1325,51 +1609,51 @@
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="16" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="17">
+      <c r="I3" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="16">
         <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="15" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="30" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="30"/>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="35" t="s">
-        <v>34</v>
+      <c r="I4" s="20" t="s">
+        <v>33</v>
       </c>
       <c r="J4" s="3">
         <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="15" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="32"/>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
@@ -1387,7 +1671,9 @@
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
+      <c r="D7" s="21" t="s">
+        <v>82</v>
+      </c>
       <c r="E7" s="21"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1404,200 +1690,226 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="C10" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
+      <c r="C11" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="C13" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="2"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="34"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="2"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="34"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="2"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="34"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="1"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="33"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C32" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="12"/>
-      <c r="E32" s="1"/>
+      <c r="E32" s="1">
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1621,17 +1933,17 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:J4"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="6"/>
     <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="24" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" style="6" customWidth="1"/>
     <col min="7" max="8" width="8.85546875" style="6"/>
     <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
     <col min="10" max="16384" width="8.85546875" style="6"/>
@@ -1656,35 +1968,37 @@
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="16" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="I3" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="16">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C4" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="30"/>
+      <c r="H4" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="20" t="s">
         <v>33</v>
-      </c>
-      <c r="J3" s="17">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C4" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="H4" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="35" t="s">
-        <v>34</v>
       </c>
       <c r="J4" s="3">
         <v>234</v>
@@ -1694,9 +2008,11 @@
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="21"/>
+      <c r="D5" s="21" t="s">
+        <v>84</v>
+      </c>
       <c r="E5" s="21"/>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
@@ -1707,9 +2023,11 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="21"/>
+      <c r="D6" s="21" t="s">
+        <v>82</v>
+      </c>
       <c r="E6" s="21"/>
-      <c r="F6" s="20"/>
+      <c r="F6" s="19"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1728,231 +2046,267 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="C10" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+    </row>
+    <row r="12" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C13" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" s="34" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="C14" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" s="34"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C32" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="18"/>
+      <c r="C32" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="12"/>
+      <c r="E32" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="F32" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="C32:E32"/>
+  <mergeCells count="8">
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>